<commit_message>
Completed FindPage. Currently working on Take Picture.
I finished FindPage, and ReceivePage also works. However, I need to finish PicturePage so I can call it when ReceivePage is done.
</commit_message>
<xml_diff>
--- a/Updated User Interface/Request Report.xlsx
+++ b/Updated User Interface/Request Report.xlsx
@@ -412,28 +412,28 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col width="21.6" customWidth="1" min="1" max="1"/>
-    <col width="14.4" customWidth="1" min="2" max="2"/>
-    <col width="16.8" customWidth="1" min="3" max="3"/>
+    <col width="14.4" customWidth="1" min="1" max="2"/>
+    <col width="25.2" customWidth="1" min="2" max="2"/>
+    <col width="88.8" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>Request ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>Report Timestamp</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Request ID</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -443,17 +443,32 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>4/13/2025, 12:00</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+      <c r="A2" t="n">
         <v>1</v>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:16:26</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Dummy Report</t>
+          <t>John Smith found battery 2. Now John Smith is Frustrated</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-04-25 10:17:01</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>John Smith received battery 2 from Battery New. Now John Smith is Tired.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Finished Implemeting Picture Frame
I've just implemented a method to take pictures while touching the screen. I've yet to integrate it to the rest of the system.
</commit_message>
<xml_diff>
--- a/Updated User Interface/Request Report.xlsx
+++ b/Updated User Interface/Request Report.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
@@ -424,55 +424,7 @@
     <col width="25.2" customWidth="1" min="2" max="2"/>
     <col width="88.8" customWidth="1" min="3" max="3"/>
   </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Request ID</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Report Timestamp</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Report</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-04-25 10:16:26</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>John Smith found battery 2. Now John Smith is Frustrated</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-04-25 10:17:01</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>John Smith received battery 2 from Battery New. Now John Smith is Tired.</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished Most of Receive
Completed Most of Receive. Implement Frame for Actions Taken and show Actions Taken in Report.
</commit_message>
<xml_diff>
--- a/Updated User Interface/Request Report.xlsx
+++ b/Updated User Interface/Request Report.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
@@ -422,9 +422,42 @@
   <cols>
     <col width="14.4" customWidth="1" min="1" max="2"/>
     <col width="25.2" customWidth="1" min="2" max="2"/>
-    <col width="88.8" customWidth="1" min="3" max="3"/>
+    <col width="68.39999999999999" customWidth="1" min="3" max="3"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Request ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Report Timestamp</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Report</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2025-04-25 19:30:06</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>John Smith found battery 2. Now John Smith is Confident</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented Receive and Ship Frames. Left with Move and Intake New Item Frames
I implemented ReceivePage and ShipPage (which are basically the same). I've got Move and Intake New Item left. Though, I think I may need a report summary page, so I'll try to implement that.
</commit_message>
<xml_diff>
--- a/Updated User Interface/Request Report.xlsx
+++ b/Updated User Interface/Request Report.xlsx
@@ -422,7 +422,7 @@
   <cols>
     <col width="14.4" customWidth="1" min="1" max="2"/>
     <col width="25.2" customWidth="1" min="2" max="2"/>
-    <col width="68.39999999999999" customWidth="1" min="3" max="3"/>
+    <col width="63.59999999999999" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -448,12 +448,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-04-25 19:30:06</t>
+          <t>2025-04-26 00:51:54</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>John Smith found battery 2. Now John Smith is Confident</t>
+          <t>John Smith found battery 2. Now John Smith is Happy</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented Every Task But "Intake New Item"
I've done everything but Intake New Item. I have Intake New Item left, but I may add a Restart Frame if needed
</commit_message>
<xml_diff>
--- a/Updated User Interface/Request Report.xlsx
+++ b/Updated User Interface/Request Report.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
@@ -422,7 +422,7 @@
   <cols>
     <col width="14.4" customWidth="1" min="1" max="2"/>
     <col width="25.2" customWidth="1" min="2" max="2"/>
-    <col width="63.59999999999999" customWidth="1" min="3" max="3"/>
+    <col width="211.2" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -448,12 +448,49 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-04-26 00:51:54</t>
+          <t>2025-04-26 06:04:32</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>John Smith found battery 2. Now John Smith is Happy</t>
+          <t>John Smith found battery 3. Now John Smith is Tired</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-04-26 06:40:03</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">John Smith received battery 2 from Suppliers Battery New.
+battery 2's state was New.
+Thus John Smith carried out the following actions:
+Store, 
+Now John Smith is Frustrated.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2025-04-26 06:50:20</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">John Smith shipped battery 2 to Suppliers Never Death Row.
+Now John Smith is Frustrated.
+</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed Excel Report Formatting
</commit_message>
<xml_diff>
--- a/Updated User Interface/Request Report.xlsx
+++ b/Updated User Interface/Request Report.xlsx
@@ -45,8 +45,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
@@ -494,6 +497,101 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>2025-04-26 11:22:52</t>
+        </is>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>John Smith found battery 2. Now John Smith is Tired</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>2025-04-26 11:24:48</t>
+        </is>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>John Smith found battery 3. Now John Smith is Confident</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>2025-04-26 11:32:09</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>John Smith found battery 2. Now John Smith is Confident</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2025-04-26 11:40:24</t>
+        </is>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">John Smith found battery 2. Now John Smith is Happy
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>2025-04-26 11:55:49</t>
+        </is>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">John Smith found battery 1. 
+ Now John Smith is Frustrated
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2025-04-26 11:59:03</t>
+        </is>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">John Smith found battery 2.
+Now John Smith is Tired
+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Move Page to handle Null Locations
</commit_message>
<xml_diff>
--- a/Updated User Interface/Request Report.xlsx
+++ b/Updated User Interface/Request Report.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
@@ -592,6 +592,36 @@
         </is>
       </c>
     </row>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2025-04-26 20:43:43</t>
+        </is>
+      </c>
+      <c r="C24" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">John Smith moved battery 7 from No Location to floor space 1.
+Now John Smith is Confident.
+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed MovePage with null location, RequestPage's picture setter, and Database's database connection method
</commit_message>
<xml_diff>
--- a/Updated User Interface/Request Report.xlsx
+++ b/Updated User Interface/Request Report.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
@@ -622,6 +622,40 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>2025-04-26 21:04:19</t>
+        </is>
+      </c>
+      <c r="C25" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">John Smith moved battery 7 from No Location to floor space 1.
+Now John Smith is Confident.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>2025-04-26 21:09:16</t>
+        </is>
+      </c>
+      <c r="C26" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">John Smith took picture of battery 7.
+Now John Smith is Happy.
+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed IntakeNewItem to also set a location
Intake New Item now connects to Move Page so that every new battery added also has a place to store it.
</commit_message>
<xml_diff>
--- a/Updated User Interface/Request Report.xlsx
+++ b/Updated User Interface/Request Report.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
@@ -656,6 +656,81 @@
         </is>
       </c>
     </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>2025-04-26 21:48:13</t>
+        </is>
+      </c>
+      <c r="C27" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">John Smith moved Its brand new from ford from No Location to shelf space 2.
+Now John Smith is Excited.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>2025-04-26 21:49:24</t>
+        </is>
+      </c>
+      <c r="C28" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">John Smith took picture of Its brand new from ford.
+Now John Smith is Frustrated.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>2025-04-26 23:34:14</t>
+        </is>
+      </c>
+      <c r="C29" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">John Smith added Nissan battery to the database.
+Serial Number is 12e12eknkndkfak.
+Part Number is 7.
+Item Type is 3.
+Now John Smith is Confident.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>2025-04-26 23:43:17</t>
+        </is>
+      </c>
+      <c r="C30" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">John Smith added Suzuki Battery to the database.
+Serial Number is 78578assa87sa87as758.
+Part Number is 9.
+Item Type is 2.
+Location is shelf space 1.
+Now John Smith is Bored.
+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
continued to make updates on appearance
</commit_message>
<xml_diff>
--- a/Updated User Interface/Request Report.xlsx
+++ b/Updated User Interface/Request Report.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
@@ -811,6 +811,41 @@
         </is>
       </c>
     </row>
+    <row r="44"/>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>44</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2025-04-28 02:08:24</t>
+        </is>
+      </c>
+      <c r="C45" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">James Davis moved Suzuki Battery from shelf space 1 to floor space 2.
+Now James Davis is Frustrated.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>45</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>2025-04-28 02:12:38</t>
+        </is>
+      </c>
+      <c r="C46" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">James Davis moved New Battery from Ford from floor space 2 to floor space 1.
+Now James Davis is Frustrated.
+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
I made more changes to the UI, tried to do madlibs style.
</commit_message>
<xml_diff>
--- a/Updated User Interface/Request Report.xlsx
+++ b/Updated User Interface/Request Report.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
@@ -425,7 +425,7 @@
   <cols>
     <col width="14.4" customWidth="1" min="1" max="2"/>
     <col width="25.2" customWidth="1" min="2" max="2"/>
-    <col width="243.6" customWidth="1" min="3" max="3"/>
+    <col width="369.6" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -846,6 +846,135 @@
         </is>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>46</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>2025-04-28 02:31:33</t>
+        </is>
+      </c>
+      <c r="C47" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">James Davis moved New Battery from Ford from floor space 2 to floor space 1.
+Now James Davis is Frustrated.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>47</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>2025-04-28 02:35:14</t>
+        </is>
+      </c>
+      <c r="C48" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">James Davis received New Battery from Ford from Suppliers Old Reliable.
+New Battery from Ford's state was New.
+Thus James Davis carried out the following actions:
+Update Battery Status, .
+Now James Davis is Tired.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>48</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>2025-04-28 02:48:44</t>
+        </is>
+      </c>
+      <c r="C49" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">James Davis moved battery 7 from floor space 1 to floor space 3.
+Now James Davis is Happy.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>49</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>2025-04-28 03:03:06</t>
+        </is>
+      </c>
+      <c r="C50" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">James Davis took picture of New Battery from Ford.
+Now James Davis is Tired, feeling that the task was Tiring.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>2025-04-28 03:05:54</t>
+        </is>
+      </c>
+      <c r="C51" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">James Davis moved New Battery from Ford from floor space 2 to floor space 2.
+Now James Davis is Confident, feeling that the task was Challenging.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>2025-04-28 03:08:10</t>
+        </is>
+      </c>
+      <c r="C52" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">James Davis received Its brand new from ford from Suppliers Battery New.
+Its brand new from ford's state was Old.
+Thus James Davis carried out the following actions:
+Update Battery Status, Diagnostic Analysis, Disassembly, Repair, Re-assembly, .
+Now James Davis is Tired, feeling that the task was Tiring.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>2025-04-28 03:10:04</t>
+        </is>
+      </c>
+      <c r="C53" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">James Davis added Telsla Battery 4 to the database.
+Serial Number is 573432019330921.
+Part Number is 3322.
+Item Type is 3.
+Location is floor space 1.
+Now James Davis is Frustrated, feeling that the task was Challenging.
+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Tried to squeeze userpage
</commit_message>
<xml_diff>
--- a/Updated User Interface/Request Report.xlsx
+++ b/Updated User Interface/Request Report.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
@@ -975,6 +975,24 @@
         </is>
       </c>
     </row>
+    <row r="54"/>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>2025-04-28 03:36:03</t>
+        </is>
+      </c>
+      <c r="C55" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">James Davis shipped New Battery from Ford to Suppliers Old Reliable.
+Now James Davis is Confident, feeling that the task was Challenging.
+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Made refinements for size on most classes
</commit_message>
<xml_diff>
--- a/Updated User Interface/Request Report.xlsx
+++ b/Updated User Interface/Request Report.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
@@ -993,6 +993,139 @@
         </is>
       </c>
     </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>2025-04-28 04:42:23</t>
+        </is>
+      </c>
+      <c r="C56" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">James Davis received Telsla Battery 4 from Suppliers Battery New.
+Telsla Battery 4's state was New.
+Thus James Davis carried out the following actions:
+Store, .
+Now James Davis is Tired, feeling that the task was Challenging.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>2025-04-28 04:43:56</t>
+        </is>
+      </c>
+      <c r="C57" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">James Davis found New Battery from Ford.
+Now James Davis is Excited, feeling that the task was Challenging.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>2025-04-28 04:54:31</t>
+        </is>
+      </c>
+      <c r="C58" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">James Davis added Brand new battery to the database.
+Serial Number is 58t3952310422.
+Part Number is 34.
+Item Type is 1231.
+Location is floor space 3.
+Now James Davis is Excited, feeling that the task was Stressful.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>2025-04-28 04:57:23</t>
+        </is>
+      </c>
+      <c r="C59" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">James Davis moved New Battery from Ford from floor space 2 to floor space 2.
+Now James Davis is Happy, feeling that the task was Fun.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>2025-04-28 05:04:55</t>
+        </is>
+      </c>
+      <c r="C60" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">James Davis received New Battery from Ford from Suppliers Never Death Row.
+New Battery from Ford's state was New.
+Thus James Davis carried out the following actions:
+Update Battery Status, Store, .
+Now James Davis is Excited, feeling that the task was Fun.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>60</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>2025-04-28 05:11:02</t>
+        </is>
+      </c>
+      <c r="C61" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">James Davis took picture of Telsla Battery 4.
+Now James Davis is Excited, feeling that the task was Rewarding.
+</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>61</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>2025-04-28 05:25:32</t>
+        </is>
+      </c>
+      <c r="C62" s="1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">James Davis added Tesla to the database.
+Serial Number: 87756453234567553
+Part Number: 54
+Item Type: 3
+Location: shelf space 1
+Now James Davis is Excited, feeling the task was Fun.
+</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Tried reducing the vertical height
</commit_message>
<xml_diff>
--- a/Updated User Interface/Request Report.xlsx
+++ b/Updated User Interface/Request Report.xlsx
@@ -1111,17 +1111,13 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2025-04-28 05:25:32</t>
+          <t>2025-04-28 05:40:23</t>
         </is>
       </c>
       <c r="C62" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">James Davis added Tesla to the database.
-Serial Number: 87756453234567553
-Part Number: 54
-Item Type: 3
-Location: shelf space 1
-Now James Davis is Excited, feeling the task was Fun.
+          <t xml:space="preserve">James Davis took a picture of New Battery from Ford.
+Now James Davis is Excited, feeling that the task was Stressful.
 </t>
         </is>
       </c>

</xml_diff>

<commit_message>
Removed The data from the debugging console
</commit_message>
<xml_diff>
--- a/Updated User Interface/Request Report.xlsx
+++ b/Updated User Interface/Request Report.xlsx
@@ -1111,13 +1111,13 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2025-04-28 05:58:51</t>
+          <t>2025-04-28 06:25:34</t>
         </is>
       </c>
       <c r="C62" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">James Davis found battery 7.
-Now James Davis is Happy, feeling that the task was Interesting.
+          <t xml:space="preserve">James Davis found New Battery from Ford.
+Now James Davis is Frustrated, feeling that the task was Stressful.
 </t>
         </is>
       </c>

</xml_diff>

<commit_message>
More commits to enhance appearance
</commit_message>
<xml_diff>
--- a/Updated User Interface/Request Report.xlsx
+++ b/Updated User Interface/Request Report.xlsx
@@ -1111,12 +1111,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2025-04-28 06:25:34</t>
+          <t>2025-04-28 06:41:58</t>
         </is>
       </c>
       <c r="C62" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">James Davis found New Battery from Ford.
+          <t xml:space="preserve">James Davis found Brand new battery.
 Now James Davis is Frustrated, feeling that the task was Stressful.
 </t>
         </is>

</xml_diff>

<commit_message>
Added startnew operation and exit feature
</commit_message>
<xml_diff>
--- a/Updated User Interface/Request Report.xlsx
+++ b/Updated User Interface/Request Report.xlsx
@@ -1111,13 +1111,13 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>2025-04-28 06:41:58</t>
+          <t>2025-04-28 16:11:39</t>
         </is>
       </c>
       <c r="C62" s="1" t="inlineStr">
         <is>
-          <t xml:space="preserve">James Davis found Brand new battery.
-Now James Davis is Frustrated, feeling that the task was Stressful.
+          <t xml:space="preserve">James Davis moved Brand new battery from floor space 3 to floor space 3.
+Now James Davis is Bored, feeling that the task was Interesting.
 </t>
         </is>
       </c>

</xml_diff>